<commit_message>
Fixed two corrupted wind gates
</commit_message>
<xml_diff>
--- a/Disks/Bugfixing/AmbermoonPatches.xlsx
+++ b/Disks/Bugfixing/AmbermoonPatches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\GitHub\Ambermoon\Disks\Bugfixing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E97BF6C-AEC6-4849-9F29-CA2BB49E91ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370EF500-2A89-431F-8126-AE3AED48C216}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fixed (Unconfirmed)" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="346">
   <si>
     <t>#</t>
   </si>
@@ -1535,6 +1535,21 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>Pyrdacor notes</t>
+  </si>
+  <si>
+    <t>After repair, left upper tile is wrong. Each of the 9 (3x3) tiles is changed by a map event with the coordinates for x and y. But the 4th event which should change the middle left tile uses y=34 instead of 35 and therefore overwrites the upper left tile. The upper-left tile is at x=9, y=34. The fix just sets the 34 to 35. :)</t>
+  </si>
+  <si>
+    <t>Y, changed byte 0x28E0 from 0x22 to 0x23 in map 231 (0xE7) inside 1Map_data.amb</t>
+  </si>
+  <si>
+    <t>Gate at 271, 563 is fine, gate at 283, 250 is missing the lower left parts. Like last issue y of one event is wrong. This time the 7th event which should change the lower left tile uses y=2 instead of 3.</t>
+  </si>
+  <si>
+    <t>Y, changed byte 0x28F6 from 0x02 to 0x03 in map 86 (0x56) inside 1Map_data.amb</t>
   </si>
 </sst>
 </file>
@@ -2177,9 +2192,9 @@
   </sheetPr>
   <dimension ref="A1:AD999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N65" sqref="N65"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9749,9 +9764,9 @@
   </sheetPr>
   <dimension ref="A1:Z1023"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9764,6 +9779,8 @@
     <col min="8" max="8" width="23.85546875" customWidth="1"/>
     <col min="9" max="9" width="81.140625" customWidth="1"/>
     <col min="10" max="10" width="61.140625" customWidth="1"/>
+    <col min="11" max="11" width="55.28515625" customWidth="1"/>
+    <col min="12" max="12" width="54.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
@@ -9797,8 +9814,12 @@
       <c r="J1" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="K1" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>339</v>
+      </c>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -10018,7 +10039,7 @@
       <c r="Y6" s="43"/>
       <c r="Z6" s="43"/>
     </row>
-    <row r="7" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A7" s="31">
         <v>6</v>
       </c>
@@ -10041,8 +10062,12 @@
         <v>251</v>
       </c>
       <c r="J7" s="53"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
+      <c r="K7" s="53" t="s">
+        <v>342</v>
+      </c>
+      <c r="L7" s="53" t="s">
+        <v>343</v>
+      </c>
       <c r="M7" s="43"/>
       <c r="N7" s="43"/>
       <c r="O7" s="43"/>
@@ -10058,7 +10083,7 @@
       <c r="Y7" s="43"/>
       <c r="Z7" s="43"/>
     </row>
-    <row r="8" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="31">
         <v>7</v>
       </c>
@@ -10081,8 +10106,12 @@
         <v>256</v>
       </c>
       <c r="J8" s="53"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
+      <c r="K8" s="53" t="s">
+        <v>344</v>
+      </c>
+      <c r="L8" s="53" t="s">
+        <v>345</v>
+      </c>
       <c r="M8" s="43"/>
       <c r="N8" s="43"/>
       <c r="O8" s="43"/>

</xml_diff>

<commit_message>
Renamed ENERGIEGLOBE to ENERGY GLOBE and fixed gadlon stairs
</commit_message>
<xml_diff>
--- a/Disks/Bugfixing/AmbermoonPatches.xlsx
+++ b/Disks/Bugfixing/AmbermoonPatches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\GitHub\Ambermoon\Disks\Bugfixing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370EF500-2A89-431F-8126-AE3AED48C216}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0488A9D8-38FA-4895-BA49-126D70EF8122}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="349">
   <si>
     <t>#</t>
   </si>
@@ -1550,6 +1550,15 @@
   </si>
   <si>
     <t>Y, changed byte 0x28F6 from 0x02 to 0x03 in map 86 (0x56) inside 1Map_data.amb</t>
+  </si>
+  <si>
+    <t>Not reproducable in english nor german versions</t>
+  </si>
+  <si>
+    <t>Won't be fixable as the palette is dependent on current window</t>
+  </si>
+  <si>
+    <t>I only found a completely missing teleport event on map 362. The stair triggers event 15 (0-based) but there are only 15 events. I added a new teleport event to map 362 which teleports to map 361 at 9,11 facing up. This feels natural in game.</t>
   </si>
 </sst>
 </file>
@@ -2193,8 +2202,8 @@
   <dimension ref="A1:AD999"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9764,9 +9773,9 @@
   </sheetPr>
   <dimension ref="A1:Z1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10152,8 +10161,12 @@
       <c r="J9" s="36" t="s">
         <v>259</v>
       </c>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
+      <c r="K9" s="43" t="s">
+        <v>346</v>
+      </c>
+      <c r="L9" s="43" t="s">
+        <v>21</v>
+      </c>
       <c r="M9" s="43"/>
       <c r="N9" s="43"/>
       <c r="O9" s="43"/>
@@ -10254,8 +10267,12 @@
         <v>260</v>
       </c>
       <c r="J12" s="53"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
+      <c r="K12" s="43" t="s">
+        <v>347</v>
+      </c>
+      <c r="L12" s="43" t="s">
+        <v>340</v>
+      </c>
       <c r="M12" s="43"/>
       <c r="N12" s="43"/>
       <c r="O12" s="43"/>
@@ -10714,8 +10731,12 @@
         <v>274</v>
       </c>
       <c r="J24" s="53"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
+      <c r="K24" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="L24" s="43" t="s">
+        <v>21</v>
+      </c>
       <c r="M24" s="43"/>
       <c r="N24" s="43"/>
       <c r="O24" s="43"/>

</xml_diff>

<commit_message>
Fixed button in bandit's cellar
</commit_message>
<xml_diff>
--- a/Disks/Bugfixing/AmbermoonPatches.xlsx
+++ b/Disks/Bugfixing/AmbermoonPatches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\GitHub\Ambermoon\Disks\Bugfixing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0488A9D8-38FA-4895-BA49-126D70EF8122}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D03F18-44C7-4370-88B2-A6DB2554F930}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="351">
   <si>
     <t>#</t>
   </si>
@@ -1559,6 +1559,12 @@
   </si>
   <si>
     <t>I only found a completely missing teleport event on map 362. The stair triggers event 15 (0-based) but there are only 15 events. I added a new teleport event to map 362 which teleports to map 361 at 9,11 facing up. This feels natural in game.</t>
+  </si>
+  <si>
+    <t>The wrong wall block is changed. Instead of 16,5 the coordinate should be 15,5.</t>
+  </si>
+  <si>
+    <t>Y, change byte at 0x0787 from 0x10 to 0x0f in map 276 in 2Map_data.amb</t>
   </si>
 </sst>
 </file>
@@ -9773,9 +9779,9 @@
   </sheetPr>
   <dimension ref="A1:Z1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10811,8 +10817,12 @@
         <v>276</v>
       </c>
       <c r="J26" s="53"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
+      <c r="K26" s="53" t="s">
+        <v>349</v>
+      </c>
+      <c r="L26" s="53" t="s">
+        <v>350</v>
+      </c>
       <c r="M26" s="43"/>
       <c r="N26" s="43"/>
       <c r="O26" s="43"/>

</xml_diff>

<commit_message>
Fixed the plants also in english version
</commit_message>
<xml_diff>
--- a/Disks/Bugfixing/AmbermoonPatches.xlsx
+++ b/Disks/Bugfixing/AmbermoonPatches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\GitHub\Ambermoon\Disks\Bugfixing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56C8FD9-76A5-4F90-AFBE-723E8972E327}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDFEFB0-9BB6-4446-812E-200A3A8CD7D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1573,13 +1573,13 @@
     <t>Works fine in remake. Needs check in original.</t>
   </si>
   <si>
-    <t>R, the best fix would be to create chests for every single flower on Kire's moon. This is a lot of work and very exhaustive without proper tools. I will leave this for later.</t>
-  </si>
-  <si>
-    <t>The problem is that some plants use the same chest index and data. So if looting one plant, the chest data becomes empty. If then another plant should be looted the code detects that the chest is already empty and as these flowers have flag "remove when empty" set, it isn't displayed anymore at all. But as the removing of the flower is done by an event chained after the chest event it will never be triggered and so the plant stays there.</t>
-  </si>
-  <si>
     <t>I only found a completely missing teleport event on map 362. The stair triggers event 15 (0-based) but there are only 15 events. I added a new teleport event to map 362 which teleports to map 361 at 9,11 facing up. This feels natural in game. Located in 3Map_data.amb</t>
+  </si>
+  <si>
+    <t>Y, many events in most maps between 300 and 335.</t>
+  </si>
+  <si>
+    <t>The event which disables the plant event chain uses the wrong index and therefore disables the plant on the wrong map. Mostly map 306, 314 and 322 are target maps. There are 1 to 4 incorrect events on many moon maps. To find the location go through map files 300 to 335 (3Map_data.amb) with a hex editor and search for hex 0E 01. This sequence starts an action event which disables a specific event afterwards. 6 bytes after the found offset there is a word (2 bytes) which gives the event bit index. Leave the last nibble (hex digit) as it is. Adjust the first 3 hex digits to the first 3 hex digits of ((MapIndex-1)*0x40) in hex. Example for map 308: (308-1)*0x40 = 4CC0. So if you find 4C42 you replace it by 4CC2.</t>
   </si>
 </sst>
 </file>
@@ -1789,7 +1789,7 @@
     <xf numFmtId="0" fontId="25" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1995,9 +1995,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9834,8 +9831,8 @@
   <dimension ref="A1:Z1023"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10792,7 +10789,7 @@
       </c>
       <c r="J24" s="53"/>
       <c r="K24" s="53" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="L24" s="79" t="s">
         <v>21</v>
@@ -11345,7 +11342,7 @@
       <c r="Y38" s="43"/>
       <c r="Z38" s="43"/>
     </row>
-    <row r="39" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A39" s="31">
         <v>39</v>
       </c>
@@ -11369,10 +11366,10 @@
       </c>
       <c r="J39" s="53"/>
       <c r="K39" s="53" t="s">
+        <v>355</v>
+      </c>
+      <c r="L39" s="80" t="s">
         <v>354</v>
-      </c>
-      <c r="L39" s="81" t="s">
-        <v>353</v>
       </c>
       <c r="M39" s="43"/>
       <c r="N39" s="43"/>

</xml_diff>

<commit_message>
Added 2 text events to Thalion office
</commit_message>
<xml_diff>
--- a/Disks/Bugfixing/AmbermoonPatches.xlsx
+++ b/Disks/Bugfixing/AmbermoonPatches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\GitHub\Ambermoon\Disks\Bugfixing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C457A480-B247-4D47-A4E3-D70B262CC9A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3619A0-963A-49E8-AF58-0EC5244213E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="364">
   <si>
     <t>#</t>
   </si>
@@ -1598,6 +1598,12 @@
   </si>
   <si>
     <t>Murderblade / dagger sling displays 0 hands but you need 1 to use</t>
+  </si>
+  <si>
+    <t>Y, added 4 events (2 for lift and 2 for stairs). One text popup and one follow up action which disables the text popup so it won't be triggered again. The lift event can be triggered by moving and eye cursor while the stair event can only be triggered by moving. I used 2 tiles in both cases. Both stair parts and both lift doors.</t>
+  </si>
+  <si>
+    <t>There were just no events for those texts at all so I added them.</t>
   </si>
 </sst>
 </file>
@@ -9851,9 +9857,9 @@
   </sheetPr>
   <dimension ref="A1:Z1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
+      <selection pane="bottomLeft" activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11535,7 +11541,7 @@
       <c r="Y42" s="43"/>
       <c r="Z42" s="43"/>
     </row>
-    <row r="43" spans="1:26" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A43" s="31">
         <v>43</v>
       </c>
@@ -11564,8 +11570,12 @@
       <c r="J43" s="36" t="s">
         <v>300</v>
       </c>
-      <c r="K43" s="43"/>
-      <c r="L43" s="43"/>
+      <c r="K43" s="43" t="s">
+        <v>363</v>
+      </c>
+      <c r="L43" s="80" t="s">
+        <v>362</v>
+      </c>
       <c r="M43" s="43"/>
       <c r="N43" s="43"/>
       <c r="O43" s="43"/>

</xml_diff>

<commit_message>
Fixed two english text bugs in Dor Grestin (Ketnar and closed shop)
</commit_message>
<xml_diff>
--- a/Disks/Bugfixing/AmbermoonPatches.xlsx
+++ b/Disks/Bugfixing/AmbermoonPatches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\GitHub\Ambermoon\Disks\Bugfixing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3619A0-963A-49E8-AF58-0EC5244213E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D45AAC1-74D8-451D-BF94-D5E5DECD7E83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="365">
   <si>
     <t>#</t>
   </si>
@@ -1604,6 +1604,9 @@
   </si>
   <si>
     <t>There were just no events for those texts at all so I added them.</t>
+  </si>
+  <si>
+    <t>Removed " |END.."</t>
   </si>
 </sst>
 </file>
@@ -9857,9 +9860,9 @@
   </sheetPr>
   <dimension ref="A1:Z1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11752,8 +11755,12 @@
       <c r="J48" s="36" t="s">
         <v>313</v>
       </c>
-      <c r="K48" s="43"/>
-      <c r="L48" s="43"/>
+      <c r="K48" s="43" t="s">
+        <v>364</v>
+      </c>
+      <c r="L48" s="43" t="s">
+        <v>21</v>
+      </c>
       <c r="M48" s="43"/>
       <c r="N48" s="43"/>
       <c r="O48" s="43"/>
@@ -11842,8 +11849,12 @@
         <v>318</v>
       </c>
       <c r="J50" s="53"/>
-      <c r="K50" s="43"/>
-      <c r="L50" s="43"/>
+      <c r="K50" s="43" t="s">
+        <v>364</v>
+      </c>
+      <c r="L50" s="43" t="s">
+        <v>21</v>
+      </c>
       <c r="M50" s="43"/>
       <c r="N50" s="43"/>
       <c r="O50" s="43"/>
@@ -11885,7 +11896,9 @@
       </c>
       <c r="J51" s="53"/>
       <c r="K51" s="43"/>
-      <c r="L51" s="43"/>
+      <c r="L51" s="43" t="s">
+        <v>21</v>
+      </c>
       <c r="M51" s="43"/>
       <c r="N51" s="43"/>
       <c r="O51" s="43"/>

</xml_diff>